<commit_message>
tests added for request demo form
</commit_message>
<xml_diff>
--- a/src/main/resources/testData/names.xlsx
+++ b/src/main/resources/testData/names.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t xml:space="preserve">pravin</t>
   </si>
@@ -44,10 +44,13 @@
     <t xml:space="preserve">password125</t>
   </si>
   <si>
+    <t xml:space="preserve">pravin ray1</t>
+  </si>
+  <si>
     <t xml:space="preserve">pravin@gmail1</t>
   </si>
   <si>
-    <t xml:space="preserve">United States</t>
+    <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">SevaDev1</t>
@@ -56,16 +59,13 @@
     <t xml:space="preserve">QA1</t>
   </si>
   <si>
-    <t xml:space="preserve">1-100</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pravin2</t>
+    <t xml:space="preserve">pravin ray2</t>
   </si>
   <si>
     <t xml:space="preserve">pravin@gmail2</t>
   </si>
   <si>
-    <t xml:space="preserve">Australia</t>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">SevaDev2</t>
@@ -74,16 +74,13 @@
     <t xml:space="preserve">QA2</t>
   </si>
   <si>
-    <t xml:space="preserve">101-500</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pravin3</t>
+    <t xml:space="preserve">pravin ray3</t>
   </si>
   <si>
     <t xml:space="preserve">pravin@gmail3</t>
   </si>
   <si>
-    <t xml:space="preserve">Nepal</t>
+    <t xml:space="preserve">3</t>
   </si>
   <si>
     <t xml:space="preserve">SevaDev3</t>
@@ -92,16 +89,13 @@
     <t xml:space="preserve">QA3</t>
   </si>
   <si>
-    <t xml:space="preserve">501-3,000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pravin4</t>
+    <t xml:space="preserve">pravin ray4</t>
   </si>
   <si>
     <t xml:space="preserve">pravin@gmail4</t>
   </si>
   <si>
-    <t xml:space="preserve">India</t>
+    <t xml:space="preserve">4</t>
   </si>
   <si>
     <t xml:space="preserve">SevaDev4</t>
@@ -110,13 +104,13 @@
     <t xml:space="preserve">QA4</t>
   </si>
   <si>
-    <t xml:space="preserve">pravin5</t>
+    <t xml:space="preserve">pravin ray5</t>
   </si>
   <si>
     <t xml:space="preserve">pravin@gmail5</t>
   </si>
   <si>
-    <t xml:space="preserve">China</t>
+    <t xml:space="preserve">5</t>
   </si>
   <si>
     <t xml:space="preserve">SevaDev5</t>
@@ -237,7 +231,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -288,38 +282,39 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="17.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="3" style="2" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="n">
         <v>987654</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -342,76 +337,76 @@
         <v>15</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>987656</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="G3" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="n">
         <v>987657</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="G4" s="2" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C5" s="2" t="n">
         <v>987658</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>